<commit_message>
chhayakhapekar: hlookup and documented for v and h lookup
</commit_message>
<xml_diff>
--- a/day-12.xlsx
+++ b/day-12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Excel\Day-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422B5016-981F-4F0E-8D1B-21CF474545AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CBF4E8-655E-486E-AB40-9D99FCEBD2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,10 +937,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712A0C3C-4B18-48EF-A398-79ADA5B682A2}">
-  <dimension ref="B3:H14"/>
+  <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="181" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:H14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="181" workbookViewId="0">
+      <selection activeCell="L7" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,22 +972,28 @@
       <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>39</v>
+      <c r="C4" s="7" t="str">
+        <f>HLOOKUP(C3,$B12:$H18,2,FALSE)</f>
+        <v>automotive sq, near tp road , 400001</v>
+      </c>
+      <c r="D4" s="7" t="str">
+        <f t="shared" ref="D4:H4" si="0">HLOOKUP(D3,$B12:$H18,2,FALSE)</f>
+        <v>offline</v>
       </c>
       <c r="E4" s="7">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F4" s="7">
+        <f t="shared" si="0"/>
         <v>5000</v>
       </c>
       <c r="G4" s="7">
+        <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="H4" s="7">
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
     </row>
@@ -995,22 +1001,28 @@
       <c r="B5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>39</v>
+      <c r="C5" s="7" t="str">
+        <f>HLOOKUP(C3,$B12:$H18,4,FALSE)</f>
+        <v>bhande plot</v>
+      </c>
+      <c r="D5" s="7" t="str">
+        <f>HLOOKUP(D3,$B12:$H18,4,FALSE)</f>
+        <v>offline</v>
       </c>
       <c r="E5" s="7">
+        <f t="shared" ref="D5:H5" si="1">HLOOKUP(E3,$B12:$H18,4,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F5" s="7">
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="G5" s="7">
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="H5" s="7">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1018,22 +1030,28 @@
       <c r="B6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>39</v>
+      <c r="C6" s="7" t="str">
+        <f>HLOOKUP(C3,$B12:$H18,5,FALSE)</f>
+        <v>jaripatka</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f t="shared" ref="D6:H6" si="2">HLOOKUP(D3,$B12:$H18,5,FALSE)</f>
+        <v>offline</v>
       </c>
       <c r="E6" s="7">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="F6" s="7">
+        <f t="shared" si="2"/>
         <v>7000</v>
       </c>
       <c r="G6" s="7">
+        <f t="shared" si="2"/>
         <v>200000</v>
       </c>
       <c r="H6" s="7">
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
     </row>
@@ -1041,22 +1059,28 @@
       <c r="B7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>40</v>
+      <c r="C7" s="7" t="str">
+        <f>HLOOKUP(C3,$B12:$H18,3,FALSE)</f>
+        <v>nandanvan</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f t="shared" ref="D7:H7" si="3">HLOOKUP(D3,$B12:$H18,3,FALSE)</f>
+        <v>online</v>
       </c>
       <c r="E7" s="7">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F7" s="7">
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
       <c r="G7" s="7">
+        <f t="shared" si="3"/>
         <v>200000</v>
       </c>
       <c r="H7" s="7">
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
     </row>
@@ -1064,22 +1088,28 @@
       <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>40</v>
+      <c r="C8" s="7" t="str">
+        <f>HLOOKUP(C3,$B12:$H18,7,FALSE)</f>
+        <v xml:space="preserve">wardhman </v>
+      </c>
+      <c r="D8" s="7" t="str">
+        <f t="shared" ref="D8:H8" si="4">HLOOKUP(D3,$B12:$H18,7,FALSE)</f>
+        <v>online</v>
       </c>
       <c r="E8" s="7">
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="F8" s="7">
+        <f t="shared" si="4"/>
         <v>12000</v>
       </c>
       <c r="G8" s="7">
+        <f t="shared" si="4"/>
         <v>150000</v>
       </c>
       <c r="H8" s="7">
+        <f t="shared" si="4"/>
         <v>7000</v>
       </c>
     </row>
@@ -1087,22 +1117,28 @@
       <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>39</v>
+      <c r="C9" s="7" t="str">
+        <f>HLOOKUP(C3,$B12:$H18,6,FALSE)</f>
+        <v>Nagpur</v>
+      </c>
+      <c r="D9" s="7" t="str">
+        <f t="shared" ref="D9:H9" si="5">HLOOKUP(D3,$B12:$H18,6,FALSE)</f>
+        <v>offline</v>
       </c>
       <c r="E9" s="7">
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="F9" s="7">
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="G9" s="7">
+        <f t="shared" si="5"/>
         <v>50000</v>
       </c>
       <c r="H9" s="7">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -1111,68 +1147,160 @@
         <v>31</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="7">
+        <v>5000</v>
+      </c>
+      <c r="D13" s="7">
+        <v>100000</v>
+      </c>
+      <c r="E13" s="7">
+        <v>700</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="H13" s="7">
         <v>5</v>
-      </c>
-      <c r="F13" s="7">
-        <v>5000</v>
-      </c>
-      <c r="G13" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H13" s="7">
-        <v>700</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="7">
+        <v>15000</v>
+      </c>
+      <c r="D14" s="7">
+        <v>200000</v>
+      </c>
+      <c r="E14" s="7">
+        <v>5000</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="7">
+        <v>10000</v>
+      </c>
+      <c r="E15" s="7">
+        <v>100</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="7">
+        <v>7000</v>
+      </c>
+      <c r="D16" s="7">
+        <v>200000</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1000</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D17" s="7">
+        <v>50000</v>
+      </c>
+      <c r="E17" s="7">
+        <v>20</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="7">
+        <v>12000</v>
+      </c>
+      <c r="D18" s="7">
+        <v>150000</v>
+      </c>
+      <c r="E18" s="7">
+        <v>7000</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7">
-        <v>15000</v>
-      </c>
-      <c r="G14" s="7">
-        <v>200000</v>
-      </c>
-      <c r="H14" s="7">
-        <v>5000</v>
+      <c r="G18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>